<commit_message>
Update ProgressKDM.xlsx revisi terbaru
</commit_message>
<xml_diff>
--- a/ProgressKDM.xlsx
+++ b/ProgressKDM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\semester 5\MAGANG BPS\KDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1D0209-CCD6-482A-B2A2-2C5EE1E4C00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB829093-5440-4AE1-9C58-697AD31555E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semua" sheetId="5" r:id="rId1"/>
@@ -364,6 +364,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -660,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90E5432-501C-4E71-A6C4-97092BA05C82}">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="101" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,13 +717,13 @@
         <v>66</v>
       </c>
       <c r="E2" s="3">
+        <v>46</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="3">
         <v>66</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="3">
-        <v>46</v>
       </c>
       <c r="H2" s="3">
         <v>20</v>
@@ -742,13 +743,13 @@
         <v>284</v>
       </c>
       <c r="E3" s="3">
+        <v>364</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="3">
         <v>520</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="3">
-        <v>364</v>
       </c>
       <c r="H3" s="3">
         <v>156</v>
@@ -794,13 +795,13 @@
         <v>77</v>
       </c>
       <c r="E5" s="3">
+        <v>75</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="3">
         <v>77</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="3">
-        <v>75</v>
       </c>
       <c r="H5" s="3">
         <v>2</v>
@@ -820,13 +821,13 @@
         <v>259</v>
       </c>
       <c r="E6" s="3">
+        <v>497</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="3">
         <v>589</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="3">
-        <v>497</v>
       </c>
       <c r="H6" s="3">
         <v>92</v>
@@ -846,13 +847,13 @@
         <v>52</v>
       </c>
       <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="3">
         <v>52</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
       </c>
       <c r="H7" s="3">
         <v>52</v>
@@ -872,13 +873,13 @@
         <v>60</v>
       </c>
       <c r="E8" s="3">
+        <v>59</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="3">
         <v>60</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="3">
-        <v>59</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
@@ -898,13 +899,13 @@
         <v>47</v>
       </c>
       <c r="E9" s="3">
+        <v>41</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="3">
         <v>47</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="3">
-        <v>41</v>
       </c>
       <c r="H9" s="3">
         <v>6</v>
@@ -950,13 +951,13 @@
         <v>13</v>
       </c>
       <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="3">
         <v>13</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
       </c>
       <c r="H11" s="3">
         <v>13</v>
@@ -1002,13 +1003,13 @@
         <v>62</v>
       </c>
       <c r="E13" s="3">
+        <v>58</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="3">
         <v>62</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="3">
-        <v>58</v>
       </c>
       <c r="H13" s="3">
         <v>4</v>
@@ -1054,13 +1055,13 @@
         <v>19</v>
       </c>
       <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="3">
         <v>19</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
       </c>
       <c r="H15" s="3">
         <v>19</v>
@@ -1106,13 +1107,13 @@
         <v>75</v>
       </c>
       <c r="E17" s="3">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>75</v>
       </c>
       <c r="G17" s="3">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="H17" s="3">
         <v>29</v>
@@ -1210,13 +1211,13 @@
         <v>10</v>
       </c>
       <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="3">
         <v>10</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0</v>
       </c>
       <c r="H21" s="3">
         <v>10</v>
@@ -1236,13 +1237,13 @@
         <v>369</v>
       </c>
       <c r="E22" s="3">
+        <v>256</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="3">
         <v>481</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="3">
-        <v>256</v>
       </c>
       <c r="H22" s="3">
         <v>225</v>
@@ -1262,13 +1263,13 @@
         <v>547</v>
       </c>
       <c r="E23" s="3">
+        <v>1005</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="3">
         <v>1192</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="3">
-        <v>1005</v>
       </c>
       <c r="H23" s="3">
         <v>187</v>
@@ -1288,13 +1289,13 @@
         <v>179</v>
       </c>
       <c r="E24" s="3">
+        <v>205</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="3">
         <v>348</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" s="3">
-        <v>205</v>
       </c>
       <c r="H24" s="3">
         <v>143</v>
@@ -1366,13 +1367,13 @@
         <v>228</v>
       </c>
       <c r="E27" s="3">
+        <v>390</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="3">
         <v>483</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="3">
-        <v>390</v>
       </c>
       <c r="H27" s="3">
         <v>93</v>
@@ -1392,13 +1393,13 @@
         <v>109</v>
       </c>
       <c r="E28" s="3">
+        <v>84</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G28" s="3">
         <v>109</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G28" s="3">
-        <v>84</v>
       </c>
       <c r="H28" s="3">
         <v>25</v>
@@ -1418,13 +1419,13 @@
         <v>4</v>
       </c>
       <c r="E29" s="3">
+        <v>2</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" s="3">
         <v>4</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G29" s="3">
-        <v>2</v>
       </c>
       <c r="H29" s="3">
         <v>2</v>
@@ -1444,13 +1445,13 @@
         <v>72</v>
       </c>
       <c r="E30" s="3">
+        <v>71</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="3">
         <v>72</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="3">
-        <v>71</v>
       </c>
       <c r="H30" s="3">
         <v>1</v>
@@ -1496,13 +1497,13 @@
         <v>367</v>
       </c>
       <c r="E32" s="3">
+        <v>675</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G32" s="3">
         <v>775</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G32" s="3">
-        <v>675</v>
       </c>
       <c r="H32" s="3">
         <v>100</v>
@@ -1652,13 +1653,13 @@
         <v>102</v>
       </c>
       <c r="E38" s="3">
+        <v>100</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G38" s="3">
         <v>102</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G38" s="3">
-        <v>100</v>
       </c>
       <c r="H38" s="3">
         <v>2</v>
@@ -1678,13 +1679,13 @@
         <v>70</v>
       </c>
       <c r="E39" s="3">
+        <v>216</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G39" s="3">
         <v>259</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G39" s="3">
-        <v>216</v>
       </c>
       <c r="H39" s="3">
         <v>43</v>
@@ -1912,13 +1913,13 @@
         <v>137</v>
       </c>
       <c r="E48" s="3">
+        <v>230</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G48" s="3">
         <v>328</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G48" s="3">
-        <v>230</v>
       </c>
       <c r="H48" s="3">
         <v>98</v>
@@ -1990,13 +1991,13 @@
         <v>30</v>
       </c>
       <c r="E51" s="3">
+        <v>29</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G51" s="3">
         <v>30</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G51" s="3">
-        <v>29</v>
       </c>
       <c r="H51" s="3">
         <v>1</v>
@@ -2016,13 +2017,13 @@
         <v>417</v>
       </c>
       <c r="E52" s="3">
+        <v>269</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G52" s="3">
         <v>586</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G52" s="3">
-        <v>269</v>
       </c>
       <c r="H52" s="3">
         <v>317</v>
@@ -2094,13 +2095,13 @@
         <v>97</v>
       </c>
       <c r="E55" s="3">
+        <v>284</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G55" s="3">
         <v>342</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G55" s="3">
-        <v>284</v>
       </c>
       <c r="H55" s="3">
         <v>58</v>
@@ -2146,13 +2147,13 @@
         <v>175</v>
       </c>
       <c r="E57" s="3">
+        <v>299</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G57" s="3">
         <v>413</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G57" s="3">
-        <v>299</v>
       </c>
       <c r="H57" s="3">
         <v>114</v>
@@ -2198,13 +2199,13 @@
         <v>275</v>
       </c>
       <c r="E59" s="3">
+        <v>106</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G59" s="3">
         <v>365</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G59" s="3">
-        <v>106</v>
       </c>
       <c r="H59" s="3">
         <v>259</v>
@@ -2224,13 +2225,13 @@
         <v>225</v>
       </c>
       <c r="E60" s="3">
+        <v>263</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G60" s="3">
         <v>406</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G60" s="3">
-        <v>263</v>
       </c>
       <c r="H60" s="3">
         <v>143</v>
@@ -2302,13 +2303,13 @@
         <v>38</v>
       </c>
       <c r="E63" s="3">
+        <v>0</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G63" s="3">
         <v>38</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G63" s="3">
-        <v>0</v>
       </c>
       <c r="H63" s="3">
         <v>38</v>
@@ -2406,13 +2407,13 @@
         <v>344</v>
       </c>
       <c r="E67" s="3">
+        <v>374</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G67" s="3">
         <v>564</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G67" s="3">
-        <v>374</v>
       </c>
       <c r="H67" s="3">
         <v>190</v>
@@ -2484,13 +2485,13 @@
         <v>56</v>
       </c>
       <c r="E70" s="3">
+        <v>28</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G70" s="3">
         <v>56</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G70" s="3">
-        <v>28</v>
       </c>
       <c r="H70" s="3">
         <v>28</v>
@@ -2510,13 +2511,13 @@
         <v>11</v>
       </c>
       <c r="E71" s="3">
+        <v>0</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G71" s="3">
         <v>11</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G71" s="3">
-        <v>0</v>
       </c>
       <c r="H71" s="3">
         <v>11</v>
@@ -2536,13 +2537,13 @@
         <v>179</v>
       </c>
       <c r="E72" s="3">
+        <v>501</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G72" s="3">
         <v>586</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G72" s="3">
-        <v>501</v>
       </c>
       <c r="H72" s="3">
         <v>85</v>
@@ -2588,13 +2589,13 @@
         <v>157</v>
       </c>
       <c r="E74" s="3">
+        <v>329</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G74" s="3">
         <v>383</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G74" s="3">
-        <v>329</v>
       </c>
       <c r="H74" s="3">
         <v>54</v>
@@ -2637,7 +2638,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2693,13 +2694,13 @@
         <v>97</v>
       </c>
       <c r="E2" s="3">
+        <v>284</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="3">
         <v>342</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="3">
-        <v>284</v>
       </c>
       <c r="H2" s="3">
         <v>58</v>
@@ -2719,13 +2720,13 @@
         <v>137</v>
       </c>
       <c r="E3" s="3">
+        <v>230</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="3">
         <v>328</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="3">
-        <v>230</v>
       </c>
       <c r="H3" s="3">
         <v>98</v>
@@ -2745,13 +2746,13 @@
         <v>284</v>
       </c>
       <c r="E4" s="3">
+        <v>364</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="3">
         <v>520</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="3">
-        <v>364</v>
       </c>
       <c r="H4" s="3">
         <v>156</v>
@@ -2771,13 +2772,13 @@
         <v>369</v>
       </c>
       <c r="E5" s="3">
+        <v>256</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="3">
         <v>481</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="3">
-        <v>256</v>
       </c>
       <c r="H5" s="3">
         <v>225</v>
@@ -2797,13 +2798,13 @@
         <v>417</v>
       </c>
       <c r="E6" s="3">
+        <v>269</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="3">
         <v>586</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="3">
-        <v>269</v>
       </c>
       <c r="H6" s="3">
         <v>317</v>
@@ -2823,13 +2824,13 @@
         <v>344</v>
       </c>
       <c r="E7" s="3">
+        <v>374</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="3">
         <v>564</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" s="3">
-        <v>374</v>
       </c>
       <c r="H7" s="3">
         <v>190</v>
@@ -2849,13 +2850,13 @@
         <v>70</v>
       </c>
       <c r="E8" s="3">
+        <v>216</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="3">
         <v>259</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="3">
-        <v>216</v>
       </c>
       <c r="H8" s="3">
         <v>43</v>
@@ -2875,13 +2876,13 @@
         <v>275</v>
       </c>
       <c r="E9" s="3">
+        <v>106</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="3">
         <v>365</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="3">
-        <v>106</v>
       </c>
       <c r="H9" s="3">
         <v>259</v>
@@ -2901,13 +2902,13 @@
         <v>259</v>
       </c>
       <c r="E10" s="3">
+        <v>497</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="3">
         <v>589</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="3">
-        <v>497</v>
       </c>
       <c r="H10" s="3">
         <v>92</v>
@@ -2927,13 +2928,13 @@
         <v>228</v>
       </c>
       <c r="E11" s="3">
+        <v>390</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="3">
         <v>483</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="3">
-        <v>390</v>
       </c>
       <c r="H11" s="3">
         <v>93</v>
@@ -2953,13 +2954,13 @@
         <v>157</v>
       </c>
       <c r="E12" s="3">
+        <v>329</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="3">
         <v>383</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" s="3">
-        <v>329</v>
       </c>
       <c r="H12" s="3">
         <v>54</v>
@@ -2979,13 +2980,13 @@
         <v>225</v>
       </c>
       <c r="E13" s="3">
+        <v>263</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="3">
         <v>406</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="3">
-        <v>263</v>
       </c>
       <c r="H13" s="3">
         <v>143</v>
@@ -3005,13 +3006,13 @@
         <v>179</v>
       </c>
       <c r="E14" s="3">
+        <v>501</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="3">
         <v>586</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" s="3">
-        <v>501</v>
       </c>
       <c r="H14" s="3">
         <v>85</v>
@@ -3031,13 +3032,13 @@
         <v>367</v>
       </c>
       <c r="E15" s="3">
+        <v>675</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="3">
         <v>775</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="3">
-        <v>675</v>
       </c>
       <c r="H15" s="3">
         <v>100</v>
@@ -3057,13 +3058,13 @@
         <v>547</v>
       </c>
       <c r="E16" s="3">
+        <v>1005</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="3">
         <v>1192</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1005</v>
       </c>
       <c r="H16" s="3">
         <v>187</v>
@@ -3083,13 +3084,13 @@
         <v>175</v>
       </c>
       <c r="E17" s="3">
+        <v>299</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="3">
         <v>413</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="3">
-        <v>299</v>
       </c>
       <c r="H17" s="3">
         <v>114</v>
@@ -3109,13 +3110,13 @@
         <v>179</v>
       </c>
       <c r="E18" s="3">
+        <v>205</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="3">
         <v>348</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="3">
-        <v>205</v>
       </c>
       <c r="H18" s="3">
         <v>143</v>
@@ -4171,8 +4172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721B1B99-A37B-47CF-BBD2-DBE8B4A5CEF5}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4224,13 +4225,13 @@
         <v>66</v>
       </c>
       <c r="E2" s="3">
+        <v>46</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="3">
         <v>66</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="3">
-        <v>46</v>
       </c>
       <c r="H2" s="3">
         <v>20</v>
@@ -4276,13 +4277,13 @@
         <v>77</v>
       </c>
       <c r="E4" s="3">
+        <v>75</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="3">
         <v>77</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="3">
-        <v>75</v>
       </c>
       <c r="H4" s="3">
         <v>2</v>
@@ -4302,13 +4303,13 @@
         <v>52</v>
       </c>
       <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="3">
         <v>52</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
       </c>
       <c r="H5" s="3">
         <v>52</v>
@@ -4328,13 +4329,13 @@
         <v>60</v>
       </c>
       <c r="E6" s="3">
+        <v>59</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="3">
         <v>60</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="3">
-        <v>59</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -4354,13 +4355,13 @@
         <v>47</v>
       </c>
       <c r="E7" s="3">
+        <v>41</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="3">
         <v>47</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" s="3">
-        <v>41</v>
       </c>
       <c r="H7" s="3">
         <v>6</v>
@@ -4406,13 +4407,13 @@
         <v>13</v>
       </c>
       <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="3">
         <v>13</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
       </c>
       <c r="H9" s="3">
         <v>13</v>
@@ -4458,13 +4459,13 @@
         <v>62</v>
       </c>
       <c r="E11" s="3">
+        <v>58</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="3">
         <v>62</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="3">
-        <v>58</v>
       </c>
       <c r="H11" s="3">
         <v>4</v>
@@ -4510,13 +4511,13 @@
         <v>19</v>
       </c>
       <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="3">
         <v>19</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0</v>
       </c>
       <c r="H13" s="3">
         <v>19</v>
@@ -4562,13 +4563,13 @@
         <v>75</v>
       </c>
       <c r="E15" s="3">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>75</v>
       </c>
       <c r="G15" s="3">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="H15" s="3">
         <v>29</v>
@@ -4666,13 +4667,13 @@
         <v>10</v>
       </c>
       <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="3">
         <v>10</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0</v>
       </c>
       <c r="H19" s="3">
         <v>10</v>
@@ -4744,13 +4745,13 @@
         <v>109</v>
       </c>
       <c r="E22" s="3">
+        <v>84</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="3">
         <v>109</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="3">
-        <v>84</v>
       </c>
       <c r="H22" s="3">
         <v>25</v>
@@ -4770,13 +4771,13 @@
         <v>4</v>
       </c>
       <c r="E23" s="3">
+        <v>2</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="3">
         <v>4</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="3">
-        <v>2</v>
       </c>
       <c r="H23" s="3">
         <v>2</v>
@@ -4796,13 +4797,13 @@
         <v>72</v>
       </c>
       <c r="E24" s="3">
+        <v>71</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" s="3">
         <v>72</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" s="3">
-        <v>71</v>
       </c>
       <c r="H24" s="3">
         <v>1</v>
@@ -4978,13 +4979,13 @@
         <v>102</v>
       </c>
       <c r="E31" s="3">
+        <v>100</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G31" s="3">
         <v>102</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G31" s="3">
-        <v>100</v>
       </c>
       <c r="H31" s="3">
         <v>2</v>
@@ -5264,13 +5265,13 @@
         <v>30</v>
       </c>
       <c r="E42" s="3">
+        <v>29</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G42" s="3">
         <v>30</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G42" s="3">
-        <v>29</v>
       </c>
       <c r="H42" s="3">
         <v>1</v>
@@ -5446,13 +5447,13 @@
         <v>38</v>
       </c>
       <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G49" s="3">
         <v>38</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G49" s="3">
-        <v>0</v>
       </c>
       <c r="H49" s="3">
         <v>38</v>
@@ -5602,13 +5603,13 @@
         <v>56</v>
       </c>
       <c r="E55" s="3">
+        <v>28</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G55" s="3">
         <v>56</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G55" s="3">
-        <v>28</v>
       </c>
       <c r="H55" s="3">
         <v>28</v>
@@ -5628,13 +5629,13 @@
         <v>11</v>
       </c>
       <c r="E56" s="3">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G56" s="3">
         <v>11</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G56" s="3">
-        <v>0</v>
       </c>
       <c r="H56" s="3">
         <v>11</v>

</xml_diff>

<commit_message>
Update app.py dan data ProgressKDM.xlsx
</commit_message>
<xml_diff>
--- a/ProgressKDM.xlsx
+++ b/ProgressKDM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\semester 5\MAGANG BPS\KDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95783DC-8CEA-4A81-86C2-5F3EF949D7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD85D7C-A195-4FC0-8504-4613A6DD3E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semua" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="110">
   <si>
     <t>Nama</t>
   </si>
@@ -355,16 +355,35 @@
   <si>
     <t>01/09/2025</t>
   </si>
+  <si>
+    <t>Nikah Nurhidayati</t>
+  </si>
+  <si>
+    <t>Eka Wahyu</t>
+  </si>
+  <si>
+    <t>Asri Ermawati</t>
+  </si>
+  <si>
+    <t>08/09/2025</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -438,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -461,71 +480,67 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90E5432-501C-4E71-A6C4-97092BA05C82}">
-  <dimension ref="A1:H218"/>
+  <dimension ref="A1:H298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="101" workbookViewId="0">
-      <selection activeCell="F217" sqref="F217"/>
+    <sheetView topLeftCell="A285" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A302" sqref="A302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6427,6 +6442,2086 @@
         <v>0</v>
       </c>
     </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A219" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B219" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C219" s="24">
+        <v>0</v>
+      </c>
+      <c r="D219" s="24">
+        <v>11</v>
+      </c>
+      <c r="E219" s="24">
+        <v>11</v>
+      </c>
+      <c r="F219" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G219" s="24">
+        <v>11</v>
+      </c>
+      <c r="H219" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A220" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B220" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C220" s="24">
+        <v>0</v>
+      </c>
+      <c r="D220" s="24">
+        <v>0</v>
+      </c>
+      <c r="E220" s="24">
+        <v>0</v>
+      </c>
+      <c r="F220" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G220" s="24">
+        <v>0</v>
+      </c>
+      <c r="H220" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A221" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B221" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C221" s="24">
+        <v>0</v>
+      </c>
+      <c r="D221" s="24">
+        <v>126</v>
+      </c>
+      <c r="E221" s="24">
+        <v>65</v>
+      </c>
+      <c r="F221" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G221" s="24">
+        <v>126</v>
+      </c>
+      <c r="H221" s="24">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A222" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B222" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C222" s="24">
+        <v>0</v>
+      </c>
+      <c r="D222" s="24">
+        <v>13</v>
+      </c>
+      <c r="E222" s="24">
+        <v>0</v>
+      </c>
+      <c r="F222" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G222" s="24">
+        <v>13</v>
+      </c>
+      <c r="H222" s="24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A223" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B223" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C223" s="24">
+        <v>0</v>
+      </c>
+      <c r="D223" s="24">
+        <v>97</v>
+      </c>
+      <c r="E223" s="24">
+        <v>97</v>
+      </c>
+      <c r="F223" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G223" s="24">
+        <v>97</v>
+      </c>
+      <c r="H223" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A224" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B224" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C224" s="24">
+        <v>0</v>
+      </c>
+      <c r="D224" s="24">
+        <v>3</v>
+      </c>
+      <c r="E224" s="24">
+        <v>0</v>
+      </c>
+      <c r="F224" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G224" s="24">
+        <v>3</v>
+      </c>
+      <c r="H224" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A225" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B225" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C225" s="24">
+        <v>0</v>
+      </c>
+      <c r="D225" s="24">
+        <v>40</v>
+      </c>
+      <c r="E225" s="24">
+        <v>40</v>
+      </c>
+      <c r="F225" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G225" s="24">
+        <v>40</v>
+      </c>
+      <c r="H225" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A226" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B226" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C226" s="24">
+        <v>0</v>
+      </c>
+      <c r="D226" s="24">
+        <v>28</v>
+      </c>
+      <c r="E226" s="24">
+        <v>28</v>
+      </c>
+      <c r="F226" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G226" s="24">
+        <v>28</v>
+      </c>
+      <c r="H226" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A227" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B227" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C227" s="26">
+        <v>90</v>
+      </c>
+      <c r="D227" s="26">
+        <v>360</v>
+      </c>
+      <c r="E227" s="26">
+        <v>449</v>
+      </c>
+      <c r="F227" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G227" s="26">
+        <v>450</v>
+      </c>
+      <c r="H227" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A228" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B228" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C228" s="24">
+        <v>0</v>
+      </c>
+      <c r="D228" s="24">
+        <v>91</v>
+      </c>
+      <c r="E228" s="24">
+        <v>91</v>
+      </c>
+      <c r="F228" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G228" s="24">
+        <v>91</v>
+      </c>
+      <c r="H228" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A229" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B229" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C229" s="24">
+        <v>0</v>
+      </c>
+      <c r="D229" s="24">
+        <v>103</v>
+      </c>
+      <c r="E229" s="24">
+        <v>103</v>
+      </c>
+      <c r="F229" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G229" s="24">
+        <v>103</v>
+      </c>
+      <c r="H229" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A230" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B230" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C230" s="26">
+        <v>189</v>
+      </c>
+      <c r="D230" s="26">
+        <v>140</v>
+      </c>
+      <c r="E230" s="26">
+        <v>320</v>
+      </c>
+      <c r="F230" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G230" s="26">
+        <v>329</v>
+      </c>
+      <c r="H230" s="26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A231" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B231" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C231" s="24">
+        <v>0</v>
+      </c>
+      <c r="D231" s="24">
+        <v>11</v>
+      </c>
+      <c r="E231" s="24">
+        <v>6</v>
+      </c>
+      <c r="F231" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G231" s="24">
+        <v>11</v>
+      </c>
+      <c r="H231" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A232" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B232" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C232" s="24">
+        <v>0</v>
+      </c>
+      <c r="D232" s="24">
+        <v>0</v>
+      </c>
+      <c r="E232" s="24">
+        <v>0</v>
+      </c>
+      <c r="F232" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G232" s="24">
+        <v>0</v>
+      </c>
+      <c r="H232" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A233" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B233" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C233" s="24">
+        <v>0</v>
+      </c>
+      <c r="D233" s="24">
+        <v>5</v>
+      </c>
+      <c r="E233" s="24">
+        <v>5</v>
+      </c>
+      <c r="F233" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G233" s="24">
+        <v>5</v>
+      </c>
+      <c r="H233" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A234" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B234" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C234" s="24">
+        <v>0</v>
+      </c>
+      <c r="D234" s="24">
+        <v>54</v>
+      </c>
+      <c r="E234" s="24">
+        <v>47</v>
+      </c>
+      <c r="F234" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G234" s="24">
+        <v>54</v>
+      </c>
+      <c r="H234" s="24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A235" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B235" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C235" s="24">
+        <v>0</v>
+      </c>
+      <c r="D235" s="24">
+        <v>88</v>
+      </c>
+      <c r="E235" s="24">
+        <v>77</v>
+      </c>
+      <c r="F235" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G235" s="24">
+        <v>88</v>
+      </c>
+      <c r="H235" s="24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A236" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B236" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C236" s="24">
+        <v>0</v>
+      </c>
+      <c r="D236" s="24">
+        <v>162</v>
+      </c>
+      <c r="E236" s="24">
+        <v>105</v>
+      </c>
+      <c r="F236" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G236" s="24">
+        <v>162</v>
+      </c>
+      <c r="H236" s="24">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A237" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B237" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C237" s="24">
+        <v>0</v>
+      </c>
+      <c r="D237" s="24">
+        <v>45</v>
+      </c>
+      <c r="E237" s="24">
+        <v>45</v>
+      </c>
+      <c r="F237" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G237" s="24">
+        <v>45</v>
+      </c>
+      <c r="H237" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A238" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B238" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C238" s="24">
+        <v>0</v>
+      </c>
+      <c r="D238" s="24">
+        <v>59</v>
+      </c>
+      <c r="E238" s="24">
+        <v>24</v>
+      </c>
+      <c r="F238" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G238" s="24">
+        <v>59</v>
+      </c>
+      <c r="H238" s="24">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A239" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B239" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C239" s="24">
+        <v>0</v>
+      </c>
+      <c r="D239" s="24">
+        <v>40</v>
+      </c>
+      <c r="E239" s="24">
+        <v>40</v>
+      </c>
+      <c r="F239" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G239" s="24">
+        <v>40</v>
+      </c>
+      <c r="H239" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A240" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B240" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C240" s="26">
+        <v>181</v>
+      </c>
+      <c r="D240" s="26">
+        <v>285</v>
+      </c>
+      <c r="E240" s="26">
+        <v>466</v>
+      </c>
+      <c r="F240" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G240" s="26">
+        <v>466</v>
+      </c>
+      <c r="H240" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A241" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B241" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C241" s="24">
+        <v>0</v>
+      </c>
+      <c r="D241" s="24">
+        <v>167</v>
+      </c>
+      <c r="E241" s="24">
+        <v>115</v>
+      </c>
+      <c r="F241" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G241" s="24">
+        <v>167</v>
+      </c>
+      <c r="H241" s="24">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A242" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B242" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C242" s="24">
+        <v>0</v>
+      </c>
+      <c r="D242" s="24">
+        <v>107</v>
+      </c>
+      <c r="E242" s="24">
+        <v>95</v>
+      </c>
+      <c r="F242" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G242" s="24">
+        <v>107</v>
+      </c>
+      <c r="H242" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A243" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B243" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C243" s="24">
+        <v>0</v>
+      </c>
+      <c r="D243" s="24">
+        <v>45</v>
+      </c>
+      <c r="E243" s="24">
+        <v>45</v>
+      </c>
+      <c r="F243" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G243" s="24">
+        <v>45</v>
+      </c>
+      <c r="H243" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A244" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B244" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C244" s="24">
+        <v>0</v>
+      </c>
+      <c r="D244" s="24">
+        <v>32</v>
+      </c>
+      <c r="E244" s="24">
+        <v>32</v>
+      </c>
+      <c r="F244" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G244" s="24">
+        <v>32</v>
+      </c>
+      <c r="H244" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A245" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B245" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C245" s="26">
+        <v>169</v>
+      </c>
+      <c r="D245" s="26">
+        <v>268</v>
+      </c>
+      <c r="E245" s="26">
+        <v>435</v>
+      </c>
+      <c r="F245" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G245" s="26">
+        <v>437</v>
+      </c>
+      <c r="H245" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A246" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B246" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C246" s="26">
+        <v>330</v>
+      </c>
+      <c r="D246" s="26">
+        <v>350</v>
+      </c>
+      <c r="E246" s="26">
+        <v>680</v>
+      </c>
+      <c r="F246" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G246" s="26">
+        <v>680</v>
+      </c>
+      <c r="H246" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A247" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B247" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C247" s="24">
+        <v>0</v>
+      </c>
+      <c r="D247" s="24">
+        <v>82</v>
+      </c>
+      <c r="E247" s="24">
+        <v>19</v>
+      </c>
+      <c r="F247" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G247" s="24">
+        <v>82</v>
+      </c>
+      <c r="H247" s="24">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A248" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B248" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C248" s="24">
+        <v>0</v>
+      </c>
+      <c r="D248" s="24">
+        <v>66</v>
+      </c>
+      <c r="E248" s="24">
+        <v>66</v>
+      </c>
+      <c r="F248" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G248" s="24">
+        <v>66</v>
+      </c>
+      <c r="H248" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A249" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B249" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C249" s="24">
+        <v>0</v>
+      </c>
+      <c r="D249" s="24">
+        <v>103</v>
+      </c>
+      <c r="E249" s="24">
+        <v>89</v>
+      </c>
+      <c r="F249" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G249" s="24">
+        <v>103</v>
+      </c>
+      <c r="H249" s="24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A250" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B250" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C250" s="26">
+        <v>238</v>
+      </c>
+      <c r="D250" s="26">
+        <v>296</v>
+      </c>
+      <c r="E250" s="26">
+        <v>534</v>
+      </c>
+      <c r="F250" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G250" s="26">
+        <v>534</v>
+      </c>
+      <c r="H250" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A251" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B251" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C251" s="24">
+        <v>0</v>
+      </c>
+      <c r="D251" s="24">
+        <v>69</v>
+      </c>
+      <c r="E251" s="24">
+        <v>60</v>
+      </c>
+      <c r="F251" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G251" s="24">
+        <v>69</v>
+      </c>
+      <c r="H251" s="24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A252" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B252" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C252" s="24">
+        <v>0</v>
+      </c>
+      <c r="D252" s="24">
+        <v>132</v>
+      </c>
+      <c r="E252" s="24">
+        <v>132</v>
+      </c>
+      <c r="F252" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G252" s="24">
+        <v>132</v>
+      </c>
+      <c r="H252" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A253" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B253" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C253" s="24">
+        <v>0</v>
+      </c>
+      <c r="D253" s="24">
+        <v>62</v>
+      </c>
+      <c r="E253" s="24">
+        <v>62</v>
+      </c>
+      <c r="F253" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G253" s="24">
+        <v>62</v>
+      </c>
+      <c r="H253" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A254" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B254" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C254" s="26">
+        <v>112</v>
+      </c>
+      <c r="D254" s="26">
+        <v>425</v>
+      </c>
+      <c r="E254" s="26">
+        <v>537</v>
+      </c>
+      <c r="F254" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G254" s="26">
+        <v>537</v>
+      </c>
+      <c r="H254" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A255" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B255" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C255" s="24">
+        <v>0</v>
+      </c>
+      <c r="D255" s="24">
+        <v>24</v>
+      </c>
+      <c r="E255" s="24">
+        <v>4</v>
+      </c>
+      <c r="F255" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G255" s="24">
+        <v>24</v>
+      </c>
+      <c r="H255" s="24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A256" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B256" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C256" s="26">
+        <v>645</v>
+      </c>
+      <c r="D256" s="26">
+        <v>656</v>
+      </c>
+      <c r="E256" s="26">
+        <v>1214</v>
+      </c>
+      <c r="F256" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G256" s="26">
+        <v>1301</v>
+      </c>
+      <c r="H256" s="26">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A257" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B257" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C257" s="26">
+        <v>407</v>
+      </c>
+      <c r="D257" s="26">
+        <v>397</v>
+      </c>
+      <c r="E257" s="26">
+        <v>814</v>
+      </c>
+      <c r="F257" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G257" s="26">
+        <v>804</v>
+      </c>
+      <c r="H257" s="26">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A258" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B258" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C258" s="24">
+        <v>0</v>
+      </c>
+      <c r="D258" s="24">
+        <v>109</v>
+      </c>
+      <c r="E258" s="24">
+        <v>109</v>
+      </c>
+      <c r="F258" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G258" s="24">
+        <v>109</v>
+      </c>
+      <c r="H258" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A259" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B259" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C259" s="24">
+        <v>0</v>
+      </c>
+      <c r="D259" s="24">
+        <v>44</v>
+      </c>
+      <c r="E259" s="24">
+        <v>36</v>
+      </c>
+      <c r="F259" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G259" s="24">
+        <v>44</v>
+      </c>
+      <c r="H259" s="24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A260" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B260" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C260" s="24">
+        <v>0</v>
+      </c>
+      <c r="D260" s="24">
+        <v>85</v>
+      </c>
+      <c r="E260" s="24">
+        <v>85</v>
+      </c>
+      <c r="F260" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G260" s="24">
+        <v>85</v>
+      </c>
+      <c r="H260" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A261" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B261" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C261" s="26">
+        <v>191</v>
+      </c>
+      <c r="D261" s="26">
+        <v>232</v>
+      </c>
+      <c r="E261" s="26">
+        <v>423</v>
+      </c>
+      <c r="F261" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G261" s="26">
+        <v>423</v>
+      </c>
+      <c r="H261" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A262" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B262" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C262" s="26">
+        <v>226</v>
+      </c>
+      <c r="D262" s="26">
+        <v>325</v>
+      </c>
+      <c r="E262" s="26">
+        <v>551</v>
+      </c>
+      <c r="F262" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G262" s="26">
+        <v>551</v>
+      </c>
+      <c r="H262" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A263" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B263" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C263" s="24">
+        <v>0</v>
+      </c>
+      <c r="D263" s="24">
+        <v>0</v>
+      </c>
+      <c r="E263" s="24">
+        <v>0</v>
+      </c>
+      <c r="F263" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G263" s="24">
+        <v>0</v>
+      </c>
+      <c r="H263" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A264" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B264" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C264" s="24">
+        <v>0</v>
+      </c>
+      <c r="D264" s="24">
+        <v>37</v>
+      </c>
+      <c r="E264" s="24">
+        <v>37</v>
+      </c>
+      <c r="F264" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G264" s="24">
+        <v>37</v>
+      </c>
+      <c r="H264" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A265" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B265" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C265" s="24">
+        <v>0</v>
+      </c>
+      <c r="D265" s="24">
+        <v>162</v>
+      </c>
+      <c r="E265" s="24">
+        <v>162</v>
+      </c>
+      <c r="F265" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G265" s="24">
+        <v>162</v>
+      </c>
+      <c r="H265" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A266" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B266" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C266" s="24">
+        <v>0</v>
+      </c>
+      <c r="D266" s="24">
+        <v>102</v>
+      </c>
+      <c r="E266" s="24">
+        <v>102</v>
+      </c>
+      <c r="F266" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G266" s="24">
+        <v>102</v>
+      </c>
+      <c r="H266" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A267" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B267" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C267" s="24">
+        <v>0</v>
+      </c>
+      <c r="D267" s="24">
+        <v>7</v>
+      </c>
+      <c r="E267" s="24">
+        <v>7</v>
+      </c>
+      <c r="F267" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G267" s="24">
+        <v>7</v>
+      </c>
+      <c r="H267" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A268" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B268" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C268" s="24">
+        <v>0</v>
+      </c>
+      <c r="D268" s="24">
+        <v>0</v>
+      </c>
+      <c r="E268" s="24">
+        <v>0</v>
+      </c>
+      <c r="F268" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G268" s="24">
+        <v>0</v>
+      </c>
+      <c r="H268" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A269" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B269" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C269" s="24">
+        <v>0</v>
+      </c>
+      <c r="D269" s="24">
+        <v>0</v>
+      </c>
+      <c r="E269" s="24">
+        <v>0</v>
+      </c>
+      <c r="F269" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G269" s="24">
+        <v>0</v>
+      </c>
+      <c r="H269" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A270" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B270" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C270" s="24">
+        <v>0</v>
+      </c>
+      <c r="D270" s="24">
+        <v>99</v>
+      </c>
+      <c r="E270" s="24">
+        <v>99</v>
+      </c>
+      <c r="F270" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G270" s="24">
+        <v>99</v>
+      </c>
+      <c r="H270" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A271" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B271" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C271" s="24">
+        <v>0</v>
+      </c>
+      <c r="D271" s="24">
+        <v>1</v>
+      </c>
+      <c r="E271" s="24">
+        <v>0</v>
+      </c>
+      <c r="F271" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G271" s="24">
+        <v>1</v>
+      </c>
+      <c r="H271" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A272" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B272" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C272" s="24">
+        <v>0</v>
+      </c>
+      <c r="D272" s="24">
+        <v>77</v>
+      </c>
+      <c r="E272" s="24">
+        <v>77</v>
+      </c>
+      <c r="F272" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G272" s="24">
+        <v>77</v>
+      </c>
+      <c r="H272" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A273" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B273" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C273" s="24">
+        <v>0</v>
+      </c>
+      <c r="D273" s="24">
+        <v>61</v>
+      </c>
+      <c r="E273" s="24">
+        <v>61</v>
+      </c>
+      <c r="F273" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G273" s="24">
+        <v>61</v>
+      </c>
+      <c r="H273" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A274" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B274" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C274" s="24">
+        <v>0</v>
+      </c>
+      <c r="D274" s="24">
+        <v>35</v>
+      </c>
+      <c r="E274" s="24">
+        <v>35</v>
+      </c>
+      <c r="F274" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G274" s="24">
+        <v>35</v>
+      </c>
+      <c r="H274" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A275" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B275" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C275" s="24">
+        <v>0</v>
+      </c>
+      <c r="D275" s="24">
+        <v>75</v>
+      </c>
+      <c r="E275" s="24">
+        <v>75</v>
+      </c>
+      <c r="F275" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G275" s="24">
+        <v>75</v>
+      </c>
+      <c r="H275" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A276" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B276" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C276" s="26">
+        <v>169</v>
+      </c>
+      <c r="D276" s="26">
+        <v>426</v>
+      </c>
+      <c r="E276" s="26">
+        <v>595</v>
+      </c>
+      <c r="F276" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G276" s="26">
+        <v>595</v>
+      </c>
+      <c r="H276" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A277" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B277" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C277" s="26">
+        <v>255</v>
+      </c>
+      <c r="D277" s="26">
+        <v>320</v>
+      </c>
+      <c r="E277" s="26">
+        <v>574</v>
+      </c>
+      <c r="F277" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G277" s="26">
+        <v>575</v>
+      </c>
+      <c r="H277" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A278" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B278" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C278" s="24">
+        <v>0</v>
+      </c>
+      <c r="D278" s="24">
+        <v>38</v>
+      </c>
+      <c r="E278" s="24">
+        <v>38</v>
+      </c>
+      <c r="F278" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G278" s="24">
+        <v>38</v>
+      </c>
+      <c r="H278" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A279" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B279" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C279" s="26">
+        <v>220</v>
+      </c>
+      <c r="D279" s="26">
+        <v>512</v>
+      </c>
+      <c r="E279" s="26">
+        <v>649</v>
+      </c>
+      <c r="F279" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G279" s="26">
+        <v>732</v>
+      </c>
+      <c r="H279" s="26">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A280" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B280" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C280" s="24">
+        <v>0</v>
+      </c>
+      <c r="D280" s="24">
+        <v>90</v>
+      </c>
+      <c r="E280" s="24">
+        <v>90</v>
+      </c>
+      <c r="F280" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G280" s="24">
+        <v>90</v>
+      </c>
+      <c r="H280" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A281" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B281" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C281" s="24">
+        <v>0</v>
+      </c>
+      <c r="D281" s="24">
+        <v>20</v>
+      </c>
+      <c r="E281" s="24">
+        <v>18</v>
+      </c>
+      <c r="F281" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G281" s="24">
+        <v>20</v>
+      </c>
+      <c r="H281" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A282" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B282" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C282" s="26">
+        <v>408</v>
+      </c>
+      <c r="D282" s="26">
+        <v>644</v>
+      </c>
+      <c r="E282" s="26">
+        <v>998</v>
+      </c>
+      <c r="F282" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G282" s="26">
+        <v>1052</v>
+      </c>
+      <c r="H282" s="26">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A283" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B283" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C283" s="24">
+        <v>0</v>
+      </c>
+      <c r="D283" s="24">
+        <v>105</v>
+      </c>
+      <c r="E283" s="24">
+        <v>105</v>
+      </c>
+      <c r="F283" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G283" s="24">
+        <v>105</v>
+      </c>
+      <c r="H283" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A284" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B284" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C284" s="24">
+        <v>0</v>
+      </c>
+      <c r="D284" s="24">
+        <v>45</v>
+      </c>
+      <c r="E284" s="24">
+        <v>45</v>
+      </c>
+      <c r="F284" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G284" s="24">
+        <v>45</v>
+      </c>
+      <c r="H284" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A285" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B285" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C285" s="24">
+        <v>0</v>
+      </c>
+      <c r="D285" s="24">
+        <v>65</v>
+      </c>
+      <c r="E285" s="24">
+        <v>64</v>
+      </c>
+      <c r="F285" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G285" s="24">
+        <v>65</v>
+      </c>
+      <c r="H285" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A286" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B286" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C286" s="24">
+        <v>0</v>
+      </c>
+      <c r="D286" s="24">
+        <v>73</v>
+      </c>
+      <c r="E286" s="24">
+        <v>73</v>
+      </c>
+      <c r="F286" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G286" s="24">
+        <v>73</v>
+      </c>
+      <c r="H286" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A287" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B287" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C287" s="24">
+        <v>0</v>
+      </c>
+      <c r="D287" s="24">
+        <v>101</v>
+      </c>
+      <c r="E287" s="24">
+        <v>0</v>
+      </c>
+      <c r="F287" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G287" s="24">
+        <v>101</v>
+      </c>
+      <c r="H287" s="24">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A288" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B288" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C288" s="24">
+        <v>0</v>
+      </c>
+      <c r="D288" s="24">
+        <v>3</v>
+      </c>
+      <c r="E288" s="24">
+        <v>0</v>
+      </c>
+      <c r="F288" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G288" s="24">
+        <v>3</v>
+      </c>
+      <c r="H288" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A289" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B289" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C289" s="24">
+        <v>0</v>
+      </c>
+      <c r="D289" s="24">
+        <v>56</v>
+      </c>
+      <c r="E289" s="24">
+        <v>56</v>
+      </c>
+      <c r="F289" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G289" s="24">
+        <v>56</v>
+      </c>
+      <c r="H289" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A290" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B290" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C290" s="24">
+        <v>0</v>
+      </c>
+      <c r="D290" s="24">
+        <v>42</v>
+      </c>
+      <c r="E290" s="24">
+        <v>42</v>
+      </c>
+      <c r="F290" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G290" s="24">
+        <v>42</v>
+      </c>
+      <c r="H290" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A291" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B291" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C291" s="26">
+        <v>245</v>
+      </c>
+      <c r="D291" s="26">
+        <v>235</v>
+      </c>
+      <c r="E291" s="26">
+        <v>474</v>
+      </c>
+      <c r="F291" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G291" s="26">
+        <v>480</v>
+      </c>
+      <c r="H291" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A292" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B292" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C292" s="24">
+        <v>0</v>
+      </c>
+      <c r="D292" s="24">
+        <v>0</v>
+      </c>
+      <c r="E292" s="24">
+        <v>0</v>
+      </c>
+      <c r="F292" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G292" s="24">
+        <v>0</v>
+      </c>
+      <c r="H292" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A293" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B293" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C293" s="24">
+        <v>0</v>
+      </c>
+      <c r="D293" s="24">
+        <v>124</v>
+      </c>
+      <c r="E293" s="24">
+        <v>87</v>
+      </c>
+      <c r="F293" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G293" s="24">
+        <v>124</v>
+      </c>
+      <c r="H293" s="24">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A294" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B294" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C294" s="24">
+        <v>0</v>
+      </c>
+      <c r="D294" s="24">
+        <v>33</v>
+      </c>
+      <c r="E294" s="24">
+        <v>33</v>
+      </c>
+      <c r="F294" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G294" s="24">
+        <v>33</v>
+      </c>
+      <c r="H294" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A295" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B295" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C295" s="24">
+        <v>0</v>
+      </c>
+      <c r="D295" s="24">
+        <v>40</v>
+      </c>
+      <c r="E295" s="24">
+        <v>18</v>
+      </c>
+      <c r="F295" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G295" s="24">
+        <v>40</v>
+      </c>
+      <c r="H295" s="24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A296" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B296" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C296" s="26">
+        <v>236</v>
+      </c>
+      <c r="D296" s="26">
+        <v>371</v>
+      </c>
+      <c r="E296" s="26">
+        <v>579</v>
+      </c>
+      <c r="F296" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G296" s="26">
+        <v>607</v>
+      </c>
+      <c r="H296" s="24">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A297" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B297" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C297" s="24">
+        <v>0</v>
+      </c>
+      <c r="D297" s="24">
+        <v>1</v>
+      </c>
+      <c r="E297" s="24">
+        <v>1</v>
+      </c>
+      <c r="F297" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G297" s="24">
+        <v>1</v>
+      </c>
+      <c r="H297" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A298" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B298" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C298" s="24">
+        <v>0</v>
+      </c>
+      <c r="D298" s="24">
+        <v>87</v>
+      </c>
+      <c r="E298" s="24">
+        <v>87</v>
+      </c>
+      <c r="F298" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G298" s="24">
+        <v>87</v>
+      </c>
+      <c r="H298" s="24">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6434,11 +8529,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H977"/>
+  <dimension ref="A1:H976"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F38" sqref="F38:F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -7806,50 +9901,619 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="24">
+        <v>90</v>
+      </c>
+      <c r="D53" s="24">
+        <v>360</v>
+      </c>
+      <c r="E53" s="24">
+        <v>449</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G53" s="24">
+        <v>450</v>
+      </c>
+      <c r="H53" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="24">
+        <v>189</v>
+      </c>
+      <c r="D54" s="24">
+        <v>140</v>
+      </c>
+      <c r="E54" s="24">
+        <v>320</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G54" s="24">
+        <v>329</v>
+      </c>
+      <c r="H54" s="24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="24">
+        <v>181</v>
+      </c>
+      <c r="D55" s="24">
+        <v>285</v>
+      </c>
+      <c r="E55" s="24">
+        <v>466</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G55" s="24">
+        <v>466</v>
+      </c>
+      <c r="H55" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="24">
+        <v>169</v>
+      </c>
+      <c r="D56" s="24">
+        <v>268</v>
+      </c>
+      <c r="E56" s="24">
+        <v>435</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G56" s="24">
+        <v>437</v>
+      </c>
+      <c r="H56" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="24">
+        <v>330</v>
+      </c>
+      <c r="D57" s="24">
+        <v>350</v>
+      </c>
+      <c r="E57" s="24">
+        <v>680</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G57" s="24">
+        <v>680</v>
+      </c>
+      <c r="H57" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="24">
+        <v>238</v>
+      </c>
+      <c r="D58" s="24">
+        <v>296</v>
+      </c>
+      <c r="E58" s="24">
+        <v>534</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G58" s="24">
+        <v>534</v>
+      </c>
+      <c r="H58" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="24">
+        <v>112</v>
+      </c>
+      <c r="D59" s="24">
+        <v>425</v>
+      </c>
+      <c r="E59" s="24">
+        <v>537</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G59" s="24">
+        <v>537</v>
+      </c>
+      <c r="H59" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="24">
+        <v>191</v>
+      </c>
+      <c r="D60" s="24">
+        <v>232</v>
+      </c>
+      <c r="E60" s="24">
+        <v>423</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G60" s="24">
+        <v>423</v>
+      </c>
+      <c r="H60" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="24">
+        <v>226</v>
+      </c>
+      <c r="D61" s="24">
+        <v>325</v>
+      </c>
+      <c r="E61" s="24">
+        <v>551</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G61" s="24">
+        <v>551</v>
+      </c>
+      <c r="H61" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B62" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="24">
+        <v>169</v>
+      </c>
+      <c r="D62" s="24">
+        <v>426</v>
+      </c>
+      <c r="E62" s="24">
+        <v>595</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G62" s="24">
+        <v>595</v>
+      </c>
+      <c r="H62" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B63" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="24">
+        <v>255</v>
+      </c>
+      <c r="D63" s="24">
+        <v>320</v>
+      </c>
+      <c r="E63" s="24">
+        <v>574</v>
+      </c>
+      <c r="F63" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G63" s="24">
+        <v>575</v>
+      </c>
+      <c r="H63" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="24">
+        <v>220</v>
+      </c>
+      <c r="D64" s="24">
+        <v>512</v>
+      </c>
+      <c r="E64" s="24">
+        <v>649</v>
+      </c>
+      <c r="F64" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G64" s="24">
+        <v>732</v>
+      </c>
+      <c r="H64" s="24">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="24">
+        <v>408</v>
+      </c>
+      <c r="D65" s="24">
+        <v>644</v>
+      </c>
+      <c r="E65" s="24">
+        <v>998</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G65" s="24">
+        <v>1052</v>
+      </c>
+      <c r="H65" s="24">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="24">
+        <v>645</v>
+      </c>
+      <c r="D66" s="24">
+        <v>656</v>
+      </c>
+      <c r="E66" s="24">
+        <v>1214</v>
+      </c>
+      <c r="F66" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G66" s="24">
+        <v>1301</v>
+      </c>
+      <c r="H66" s="24">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="24">
+        <v>407</v>
+      </c>
+      <c r="D67" s="24">
+        <v>397</v>
+      </c>
+      <c r="E67" s="24">
+        <v>814</v>
+      </c>
+      <c r="F67" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G67" s="24">
+        <v>804</v>
+      </c>
+      <c r="H67" s="24">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="24">
+        <v>245</v>
+      </c>
+      <c r="D68" s="24">
+        <v>235</v>
+      </c>
+      <c r="E68" s="24">
+        <v>474</v>
+      </c>
+      <c r="F68" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G68" s="24">
+        <v>480</v>
+      </c>
+      <c r="H68" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B69" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" s="24">
+        <v>236</v>
+      </c>
+      <c r="D69" s="24">
+        <v>371</v>
+      </c>
+      <c r="E69" s="24">
+        <v>579</v>
+      </c>
+      <c r="F69" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G69" s="24">
+        <v>607</v>
+      </c>
+      <c r="H69" s="24">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="27"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="28"/>
+      <c r="F70" s="29"/>
+      <c r="G70" s="28"/>
+      <c r="H70" s="28"/>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="27"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="28"/>
+      <c r="H71" s="28"/>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="27"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="29"/>
+      <c r="G72" s="28"/>
+      <c r="H72" s="28"/>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="29"/>
+      <c r="G73" s="28"/>
+      <c r="H73" s="28"/>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="29"/>
+      <c r="G74" s="28"/>
+      <c r="H74" s="28"/>
+    </row>
+    <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="28"/>
+    </row>
+    <row r="76" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="28"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="28"/>
+      <c r="H76" s="28"/>
+    </row>
+    <row r="77" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="28"/>
+      <c r="H77" s="28"/>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="27"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="28"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="28"/>
+      <c r="H78" s="28"/>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="27"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="28"/>
+      <c r="F79" s="29"/>
+      <c r="G79" s="28"/>
+      <c r="H79" s="28"/>
+    </row>
+    <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="28"/>
+      <c r="H80" s="28"/>
+    </row>
+    <row r="81" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="29"/>
+      <c r="G81" s="28"/>
+      <c r="H81" s="28"/>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="28"/>
+      <c r="F82" s="29"/>
+      <c r="G82" s="28"/>
+      <c r="H82" s="28"/>
+    </row>
+    <row r="83" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="29"/>
+      <c r="G83" s="28"/>
+      <c r="H83" s="28"/>
+    </row>
+    <row r="84" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="29"/>
+      <c r="G84" s="28"/>
+      <c r="H84" s="28"/>
+    </row>
+    <row r="85" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="28"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="28"/>
+      <c r="H85" s="28"/>
+    </row>
+    <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -8730,7 +11394,6 @@
     <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -8739,10 +11402,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721B1B99-A37B-47CF-BBD2-DBE8B4A5CEF5}">
-  <dimension ref="A1:H173"/>
+  <dimension ref="A1:H230"/>
   <sheetViews>
-    <sheetView topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="F135" sqref="F135:F150"/>
+    <sheetView topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="B227" sqref="B227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13086,7 +15749,7 @@
       <c r="E167" s="17">
         <v>60</v>
       </c>
-      <c r="F167" s="21" t="s">
+      <c r="F167" s="20" t="s">
         <v>105</v>
       </c>
       <c r="G167" s="17">
@@ -13097,22 +15760,1642 @@
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F168" s="23"/>
+      <c r="A168" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B168" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C168" s="24">
+        <v>0</v>
+      </c>
+      <c r="D168" s="24">
+        <v>11</v>
+      </c>
+      <c r="E168" s="24">
+        <v>11</v>
+      </c>
+      <c r="F168" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G168" s="24">
+        <v>11</v>
+      </c>
+      <c r="H168" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F169" s="22"/>
+      <c r="A169" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B169" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C169" s="24">
+        <v>0</v>
+      </c>
+      <c r="D169" s="24">
+        <v>0</v>
+      </c>
+      <c r="E169" s="24">
+        <v>0</v>
+      </c>
+      <c r="F169" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G169" s="24">
+        <v>0</v>
+      </c>
+      <c r="H169" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F170" s="22"/>
+      <c r="A170" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B170" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C170" s="24">
+        <v>0</v>
+      </c>
+      <c r="D170" s="24">
+        <v>126</v>
+      </c>
+      <c r="E170" s="24">
+        <v>65</v>
+      </c>
+      <c r="F170" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G170" s="24">
+        <v>126</v>
+      </c>
+      <c r="H170" s="24">
+        <v>61</v>
+      </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F171" s="22"/>
+      <c r="A171" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B171" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C171" s="24">
+        <v>0</v>
+      </c>
+      <c r="D171" s="24">
+        <v>13</v>
+      </c>
+      <c r="E171" s="24">
+        <v>0</v>
+      </c>
+      <c r="F171" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G171" s="24">
+        <v>13</v>
+      </c>
+      <c r="H171" s="24">
+        <v>13</v>
+      </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F172" s="22"/>
+      <c r="A172" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B172" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C172" s="24">
+        <v>0</v>
+      </c>
+      <c r="D172" s="24">
+        <v>97</v>
+      </c>
+      <c r="E172" s="24">
+        <v>97</v>
+      </c>
+      <c r="F172" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G172" s="24">
+        <v>97</v>
+      </c>
+      <c r="H172" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F173" s="22"/>
+      <c r="A173" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B173" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C173" s="24">
+        <v>0</v>
+      </c>
+      <c r="D173" s="24">
+        <v>3</v>
+      </c>
+      <c r="E173" s="24">
+        <v>0</v>
+      </c>
+      <c r="F173" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G173" s="24">
+        <v>3</v>
+      </c>
+      <c r="H173" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A174" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B174" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C174" s="24">
+        <v>0</v>
+      </c>
+      <c r="D174" s="24">
+        <v>40</v>
+      </c>
+      <c r="E174" s="24">
+        <v>40</v>
+      </c>
+      <c r="F174" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G174" s="24">
+        <v>40</v>
+      </c>
+      <c r="H174" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A175" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B175" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C175" s="24">
+        <v>0</v>
+      </c>
+      <c r="D175" s="24">
+        <v>28</v>
+      </c>
+      <c r="E175" s="24">
+        <v>28</v>
+      </c>
+      <c r="F175" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G175" s="24">
+        <v>28</v>
+      </c>
+      <c r="H175" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A176" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B176" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C176" s="24">
+        <v>0</v>
+      </c>
+      <c r="D176" s="24">
+        <v>91</v>
+      </c>
+      <c r="E176" s="24">
+        <v>91</v>
+      </c>
+      <c r="F176" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G176" s="24">
+        <v>91</v>
+      </c>
+      <c r="H176" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A177" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B177" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C177" s="24">
+        <v>0</v>
+      </c>
+      <c r="D177" s="24">
+        <v>103</v>
+      </c>
+      <c r="E177" s="24">
+        <v>103</v>
+      </c>
+      <c r="F177" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G177" s="24">
+        <v>103</v>
+      </c>
+      <c r="H177" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A178" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B178" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C178" s="24">
+        <v>0</v>
+      </c>
+      <c r="D178" s="24">
+        <v>11</v>
+      </c>
+      <c r="E178" s="24">
+        <v>6</v>
+      </c>
+      <c r="F178" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G178" s="24">
+        <v>11</v>
+      </c>
+      <c r="H178" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A179" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B179" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C179" s="24">
+        <v>0</v>
+      </c>
+      <c r="D179" s="24">
+        <v>0</v>
+      </c>
+      <c r="E179" s="24">
+        <v>0</v>
+      </c>
+      <c r="F179" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G179" s="24">
+        <v>0</v>
+      </c>
+      <c r="H179" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A180" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B180" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C180" s="24">
+        <v>0</v>
+      </c>
+      <c r="D180" s="24">
+        <v>5</v>
+      </c>
+      <c r="E180" s="24">
+        <v>5</v>
+      </c>
+      <c r="F180" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G180" s="24">
+        <v>5</v>
+      </c>
+      <c r="H180" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A181" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B181" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C181" s="24">
+        <v>0</v>
+      </c>
+      <c r="D181" s="24">
+        <v>54</v>
+      </c>
+      <c r="E181" s="24">
+        <v>47</v>
+      </c>
+      <c r="F181" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G181" s="24">
+        <v>54</v>
+      </c>
+      <c r="H181" s="24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A182" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B182" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C182" s="24">
+        <v>0</v>
+      </c>
+      <c r="D182" s="24">
+        <v>88</v>
+      </c>
+      <c r="E182" s="24">
+        <v>77</v>
+      </c>
+      <c r="F182" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G182" s="24">
+        <v>88</v>
+      </c>
+      <c r="H182" s="24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A183" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B183" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C183" s="24">
+        <v>0</v>
+      </c>
+      <c r="D183" s="24">
+        <v>162</v>
+      </c>
+      <c r="E183" s="24">
+        <v>105</v>
+      </c>
+      <c r="F183" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G183" s="24">
+        <v>162</v>
+      </c>
+      <c r="H183" s="24">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A184" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B184" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C184" s="24">
+        <v>0</v>
+      </c>
+      <c r="D184" s="24">
+        <v>45</v>
+      </c>
+      <c r="E184" s="24">
+        <v>45</v>
+      </c>
+      <c r="F184" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G184" s="24">
+        <v>45</v>
+      </c>
+      <c r="H184" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A185" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B185" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C185" s="24">
+        <v>0</v>
+      </c>
+      <c r="D185" s="24">
+        <v>59</v>
+      </c>
+      <c r="E185" s="24">
+        <v>24</v>
+      </c>
+      <c r="F185" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G185" s="24">
+        <v>59</v>
+      </c>
+      <c r="H185" s="24">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A186" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B186" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C186" s="24">
+        <v>0</v>
+      </c>
+      <c r="D186" s="24">
+        <v>40</v>
+      </c>
+      <c r="E186" s="24">
+        <v>40</v>
+      </c>
+      <c r="F186" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G186" s="24">
+        <v>40</v>
+      </c>
+      <c r="H186" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A187" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B187" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C187" s="24">
+        <v>0</v>
+      </c>
+      <c r="D187" s="24">
+        <v>167</v>
+      </c>
+      <c r="E187" s="24">
+        <v>115</v>
+      </c>
+      <c r="F187" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G187" s="24">
+        <v>167</v>
+      </c>
+      <c r="H187" s="24">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A188" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B188" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C188" s="24">
+        <v>0</v>
+      </c>
+      <c r="D188" s="24">
+        <v>107</v>
+      </c>
+      <c r="E188" s="24">
+        <v>95</v>
+      </c>
+      <c r="F188" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G188" s="24">
+        <v>107</v>
+      </c>
+      <c r="H188" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A189" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B189" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C189" s="24">
+        <v>0</v>
+      </c>
+      <c r="D189" s="24">
+        <v>45</v>
+      </c>
+      <c r="E189" s="24">
+        <v>45</v>
+      </c>
+      <c r="F189" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G189" s="24">
+        <v>45</v>
+      </c>
+      <c r="H189" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A190" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B190" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C190" s="24">
+        <v>0</v>
+      </c>
+      <c r="D190" s="24">
+        <v>32</v>
+      </c>
+      <c r="E190" s="24">
+        <v>32</v>
+      </c>
+      <c r="F190" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G190" s="24">
+        <v>32</v>
+      </c>
+      <c r="H190" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A191" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B191" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C191" s="24">
+        <v>0</v>
+      </c>
+      <c r="D191" s="24">
+        <v>82</v>
+      </c>
+      <c r="E191" s="24">
+        <v>19</v>
+      </c>
+      <c r="F191" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G191" s="24">
+        <v>82</v>
+      </c>
+      <c r="H191" s="24">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A192" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B192" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C192" s="24">
+        <v>0</v>
+      </c>
+      <c r="D192" s="24">
+        <v>66</v>
+      </c>
+      <c r="E192" s="24">
+        <v>66</v>
+      </c>
+      <c r="F192" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G192" s="24">
+        <v>66</v>
+      </c>
+      <c r="H192" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A193" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B193" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C193" s="24">
+        <v>0</v>
+      </c>
+      <c r="D193" s="24">
+        <v>103</v>
+      </c>
+      <c r="E193" s="24">
+        <v>89</v>
+      </c>
+      <c r="F193" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G193" s="24">
+        <v>103</v>
+      </c>
+      <c r="H193" s="24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A194" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B194" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C194" s="24">
+        <v>0</v>
+      </c>
+      <c r="D194" s="24">
+        <v>69</v>
+      </c>
+      <c r="E194" s="24">
+        <v>60</v>
+      </c>
+      <c r="F194" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G194" s="24">
+        <v>69</v>
+      </c>
+      <c r="H194" s="24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A195" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B195" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C195" s="24">
+        <v>0</v>
+      </c>
+      <c r="D195" s="24">
+        <v>132</v>
+      </c>
+      <c r="E195" s="24">
+        <v>132</v>
+      </c>
+      <c r="F195" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G195" s="24">
+        <v>132</v>
+      </c>
+      <c r="H195" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A196" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B196" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C196" s="24">
+        <v>0</v>
+      </c>
+      <c r="D196" s="24">
+        <v>62</v>
+      </c>
+      <c r="E196" s="24">
+        <v>62</v>
+      </c>
+      <c r="F196" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G196" s="24">
+        <v>62</v>
+      </c>
+      <c r="H196" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A197" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B197" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C197" s="24">
+        <v>0</v>
+      </c>
+      <c r="D197" s="24">
+        <v>24</v>
+      </c>
+      <c r="E197" s="24">
+        <v>4</v>
+      </c>
+      <c r="F197" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G197" s="24">
+        <v>24</v>
+      </c>
+      <c r="H197" s="24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A198" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B198" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C198" s="24">
+        <v>0</v>
+      </c>
+      <c r="D198" s="24">
+        <v>109</v>
+      </c>
+      <c r="E198" s="24">
+        <v>109</v>
+      </c>
+      <c r="F198" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G198" s="24">
+        <v>109</v>
+      </c>
+      <c r="H198" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A199" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B199" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C199" s="24">
+        <v>0</v>
+      </c>
+      <c r="D199" s="24">
+        <v>44</v>
+      </c>
+      <c r="E199" s="24">
+        <v>36</v>
+      </c>
+      <c r="F199" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G199" s="24">
+        <v>44</v>
+      </c>
+      <c r="H199" s="24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A200" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B200" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C200" s="24">
+        <v>0</v>
+      </c>
+      <c r="D200" s="24">
+        <v>85</v>
+      </c>
+      <c r="E200" s="24">
+        <v>85</v>
+      </c>
+      <c r="F200" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G200" s="24">
+        <v>85</v>
+      </c>
+      <c r="H200" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A201" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B201" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C201" s="24">
+        <v>0</v>
+      </c>
+      <c r="D201" s="24">
+        <v>0</v>
+      </c>
+      <c r="E201" s="24">
+        <v>0</v>
+      </c>
+      <c r="F201" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G201" s="24">
+        <v>0</v>
+      </c>
+      <c r="H201" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A202" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B202" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C202" s="24">
+        <v>0</v>
+      </c>
+      <c r="D202" s="24">
+        <v>37</v>
+      </c>
+      <c r="E202" s="24">
+        <v>37</v>
+      </c>
+      <c r="F202" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G202" s="24">
+        <v>37</v>
+      </c>
+      <c r="H202" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A203" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B203" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C203" s="24">
+        <v>0</v>
+      </c>
+      <c r="D203" s="24">
+        <v>162</v>
+      </c>
+      <c r="E203" s="24">
+        <v>162</v>
+      </c>
+      <c r="F203" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G203" s="24">
+        <v>162</v>
+      </c>
+      <c r="H203" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A204" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B204" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C204" s="24">
+        <v>0</v>
+      </c>
+      <c r="D204" s="24">
+        <v>102</v>
+      </c>
+      <c r="E204" s="24">
+        <v>102</v>
+      </c>
+      <c r="F204" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G204" s="24">
+        <v>102</v>
+      </c>
+      <c r="H204" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A205" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B205" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C205" s="24">
+        <v>0</v>
+      </c>
+      <c r="D205" s="24">
+        <v>7</v>
+      </c>
+      <c r="E205" s="24">
+        <v>7</v>
+      </c>
+      <c r="F205" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G205" s="24">
+        <v>7</v>
+      </c>
+      <c r="H205" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A206" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B206" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C206" s="24">
+        <v>0</v>
+      </c>
+      <c r="D206" s="24">
+        <v>0</v>
+      </c>
+      <c r="E206" s="24">
+        <v>0</v>
+      </c>
+      <c r="F206" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G206" s="24">
+        <v>0</v>
+      </c>
+      <c r="H206" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A207" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B207" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C207" s="24">
+        <v>0</v>
+      </c>
+      <c r="D207" s="24">
+        <v>0</v>
+      </c>
+      <c r="E207" s="24">
+        <v>0</v>
+      </c>
+      <c r="F207" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G207" s="24">
+        <v>0</v>
+      </c>
+      <c r="H207" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A208" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B208" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C208" s="24">
+        <v>0</v>
+      </c>
+      <c r="D208" s="24">
+        <v>99</v>
+      </c>
+      <c r="E208" s="24">
+        <v>99</v>
+      </c>
+      <c r="F208" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G208" s="24">
+        <v>99</v>
+      </c>
+      <c r="H208" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A209" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B209" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C209" s="24">
+        <v>0</v>
+      </c>
+      <c r="D209" s="24">
+        <v>1</v>
+      </c>
+      <c r="E209" s="24">
+        <v>0</v>
+      </c>
+      <c r="F209" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G209" s="24">
+        <v>1</v>
+      </c>
+      <c r="H209" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A210" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B210" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C210" s="24">
+        <v>0</v>
+      </c>
+      <c r="D210" s="24">
+        <v>77</v>
+      </c>
+      <c r="E210" s="24">
+        <v>77</v>
+      </c>
+      <c r="F210" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G210" s="24">
+        <v>77</v>
+      </c>
+      <c r="H210" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A211" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B211" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C211" s="24">
+        <v>0</v>
+      </c>
+      <c r="D211" s="24">
+        <v>61</v>
+      </c>
+      <c r="E211" s="24">
+        <v>61</v>
+      </c>
+      <c r="F211" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G211" s="24">
+        <v>61</v>
+      </c>
+      <c r="H211" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A212" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B212" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C212" s="24">
+        <v>0</v>
+      </c>
+      <c r="D212" s="24">
+        <v>35</v>
+      </c>
+      <c r="E212" s="24">
+        <v>35</v>
+      </c>
+      <c r="F212" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G212" s="24">
+        <v>35</v>
+      </c>
+      <c r="H212" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A213" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B213" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C213" s="24">
+        <v>0</v>
+      </c>
+      <c r="D213" s="24">
+        <v>75</v>
+      </c>
+      <c r="E213" s="24">
+        <v>75</v>
+      </c>
+      <c r="F213" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G213" s="24">
+        <v>75</v>
+      </c>
+      <c r="H213" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A214" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B214" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C214" s="24">
+        <v>0</v>
+      </c>
+      <c r="D214" s="24">
+        <v>38</v>
+      </c>
+      <c r="E214" s="24">
+        <v>38</v>
+      </c>
+      <c r="F214" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G214" s="24">
+        <v>38</v>
+      </c>
+      <c r="H214" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A215" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B215" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C215" s="24">
+        <v>0</v>
+      </c>
+      <c r="D215" s="24">
+        <v>90</v>
+      </c>
+      <c r="E215" s="24">
+        <v>90</v>
+      </c>
+      <c r="F215" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G215" s="24">
+        <v>90</v>
+      </c>
+      <c r="H215" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A216" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B216" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C216" s="24">
+        <v>0</v>
+      </c>
+      <c r="D216" s="24">
+        <v>20</v>
+      </c>
+      <c r="E216" s="24">
+        <v>18</v>
+      </c>
+      <c r="F216" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G216" s="24">
+        <v>20</v>
+      </c>
+      <c r="H216" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A217" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B217" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C217" s="24">
+        <v>0</v>
+      </c>
+      <c r="D217" s="24">
+        <v>105</v>
+      </c>
+      <c r="E217" s="24">
+        <v>105</v>
+      </c>
+      <c r="F217" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G217" s="24">
+        <v>105</v>
+      </c>
+      <c r="H217" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A218" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B218" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C218" s="24">
+        <v>0</v>
+      </c>
+      <c r="D218" s="24">
+        <v>45</v>
+      </c>
+      <c r="E218" s="24">
+        <v>45</v>
+      </c>
+      <c r="F218" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G218" s="24">
+        <v>45</v>
+      </c>
+      <c r="H218" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A219" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B219" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C219" s="24">
+        <v>0</v>
+      </c>
+      <c r="D219" s="24">
+        <v>65</v>
+      </c>
+      <c r="E219" s="24">
+        <v>64</v>
+      </c>
+      <c r="F219" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G219" s="24">
+        <v>65</v>
+      </c>
+      <c r="H219" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A220" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B220" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C220" s="24">
+        <v>0</v>
+      </c>
+      <c r="D220" s="24">
+        <v>73</v>
+      </c>
+      <c r="E220" s="24">
+        <v>73</v>
+      </c>
+      <c r="F220" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G220" s="24">
+        <v>73</v>
+      </c>
+      <c r="H220" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A221" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B221" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C221" s="24">
+        <v>0</v>
+      </c>
+      <c r="D221" s="24">
+        <v>101</v>
+      </c>
+      <c r="E221" s="24">
+        <v>0</v>
+      </c>
+      <c r="F221" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G221" s="24">
+        <v>101</v>
+      </c>
+      <c r="H221" s="24">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A222" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B222" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C222" s="24">
+        <v>0</v>
+      </c>
+      <c r="D222" s="24">
+        <v>3</v>
+      </c>
+      <c r="E222" s="24">
+        <v>0</v>
+      </c>
+      <c r="F222" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G222" s="24">
+        <v>3</v>
+      </c>
+      <c r="H222" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A223" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B223" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C223" s="24">
+        <v>0</v>
+      </c>
+      <c r="D223" s="24">
+        <v>56</v>
+      </c>
+      <c r="E223" s="24">
+        <v>56</v>
+      </c>
+      <c r="F223" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G223" s="24">
+        <v>56</v>
+      </c>
+      <c r="H223" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A224" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B224" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C224" s="24">
+        <v>0</v>
+      </c>
+      <c r="D224" s="24">
+        <v>42</v>
+      </c>
+      <c r="E224" s="24">
+        <v>42</v>
+      </c>
+      <c r="F224" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G224" s="24">
+        <v>42</v>
+      </c>
+      <c r="H224" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A225" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B225" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C225" s="24">
+        <v>0</v>
+      </c>
+      <c r="D225" s="24">
+        <v>0</v>
+      </c>
+      <c r="E225" s="24">
+        <v>0</v>
+      </c>
+      <c r="F225" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G225" s="24">
+        <v>0</v>
+      </c>
+      <c r="H225" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A226" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B226" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C226" s="24">
+        <v>0</v>
+      </c>
+      <c r="D226" s="24">
+        <v>124</v>
+      </c>
+      <c r="E226" s="24">
+        <v>87</v>
+      </c>
+      <c r="F226" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G226" s="24">
+        <v>124</v>
+      </c>
+      <c r="H226" s="24">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A227" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B227" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C227" s="24">
+        <v>0</v>
+      </c>
+      <c r="D227" s="24">
+        <v>33</v>
+      </c>
+      <c r="E227" s="24">
+        <v>33</v>
+      </c>
+      <c r="F227" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G227" s="24">
+        <v>33</v>
+      </c>
+      <c r="H227" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A228" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B228" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C228" s="24">
+        <v>0</v>
+      </c>
+      <c r="D228" s="24">
+        <v>40</v>
+      </c>
+      <c r="E228" s="24">
+        <v>18</v>
+      </c>
+      <c r="F228" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G228" s="24">
+        <v>40</v>
+      </c>
+      <c r="H228" s="24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A229" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B229" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C229" s="24">
+        <v>0</v>
+      </c>
+      <c r="D229" s="24">
+        <v>1</v>
+      </c>
+      <c r="E229" s="24">
+        <v>1</v>
+      </c>
+      <c r="F229" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G229" s="24">
+        <v>1</v>
+      </c>
+      <c r="H229" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A230" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B230" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C230" s="24">
+        <v>0</v>
+      </c>
+      <c r="D230" s="24">
+        <v>87</v>
+      </c>
+      <c r="E230" s="24">
+        <v>87</v>
+      </c>
+      <c r="F230" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G230" s="24">
+        <v>87</v>
+      </c>
+      <c r="H230" s="24">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>